<commit_message>
Bug eye icon screenshot added
</commit_message>
<xml_diff>
--- a/Book House.xlsx
+++ b/Book House.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="499">
   <si>
     <t>Please click here for book house testplan full PDF.</t>
   </si>
@@ -580,6 +580,7 @@
         <rFont val="Arial"/>
         <color rgb="FF000000"/>
         <sz val="11.0"/>
+        <u/>
       </rPr>
       <t xml:space="preserve">1. Goto the URL </t>
     </r>
@@ -597,18 +598,10 @@
         <rFont val="Arial"/>
         <color rgb="FF000000"/>
         <sz val="11.0"/>
+        <u/>
       </rPr>
       <t xml:space="preserve">
-2</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-        <u/>
-      </rPr>
-      <t xml:space="preserve">. Click on the "Login" button in the right corner.
+2. Click on the "Login" button in the right corner.
 3. Enter password </t>
     </r>
   </si>
@@ -2892,7 +2885,7 @@
     </r>
   </si>
   <si>
-    <t>Screenshot:</t>
+    <t>Screenshot: Eye Icon</t>
   </si>
   <si>
     <r>
@@ -3090,6 +3083,9 @@
   </si>
   <si>
     <t>Severity: minor</t>
+  </si>
+  <si>
+    <t>Screenshot:</t>
   </si>
   <si>
     <r>
@@ -3610,7 +3606,7 @@
     <font>
       <u/>
       <sz val="11.0"/>
-      <color rgb="FF0563C1"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -19362,7 +19358,7 @@
         <v>113</v>
       </c>
       <c r="H16" s="87"/>
-      <c r="I16" s="91" t="s">
+      <c r="I16" s="112" t="s">
         <v>114</v>
       </c>
       <c r="J16" s="124" t="s">
@@ -24628,12 +24624,12 @@
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="B73" s="292" t="s">
-        <v>427</v>
+        <v>449</v>
       </c>
     </row>
     <row r="74" ht="12.75" customHeight="1">
       <c r="B74" s="288" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="75" ht="12.75" customHeight="1">
@@ -24666,7 +24662,7 @@
     </row>
     <row r="83" ht="12.75" customHeight="1">
       <c r="B83" s="287" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="84" ht="12.75" customHeight="1">
@@ -24674,7 +24670,7 @@
     </row>
     <row r="85" ht="12.75" customHeight="1">
       <c r="B85" s="288" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="86" ht="12.75" customHeight="1">
@@ -24687,17 +24683,17 @@
     </row>
     <row r="88" ht="12.75" customHeight="1">
       <c r="B88" s="289" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="89" ht="12.75" customHeight="1">
       <c r="B89" s="291" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="90" ht="12.75" customHeight="1">
       <c r="B90" s="291" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="91" ht="12.75" customHeight="1">
@@ -24715,22 +24711,22 @@
     </row>
     <row r="94" ht="12.75" customHeight="1">
       <c r="B94" s="288" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="95" ht="12.75" customHeight="1">
       <c r="B95" s="288" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="96" ht="12.75" customHeight="1">
       <c r="B96" s="298" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="97" ht="12.75" customHeight="1">
       <c r="B97" s="288" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="98" ht="12.75" customHeight="1">
@@ -24761,7 +24757,7 @@
     </row>
     <row r="108" ht="12.75" customHeight="1">
       <c r="B108" s="301" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="109" ht="12.75" customHeight="1">
@@ -24769,7 +24765,7 @@
     </row>
     <row r="110" ht="12.75" customHeight="1">
       <c r="B110" s="301" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="111" ht="12.75" customHeight="1">
@@ -24782,17 +24778,17 @@
     </row>
     <row r="113" ht="12.75" customHeight="1">
       <c r="B113" s="304" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="114" ht="12.75" customHeight="1">
       <c r="B114" s="305" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="115" ht="12.75" customHeight="1">
       <c r="B115" s="305" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="116" ht="12.75" customHeight="1">
@@ -24805,17 +24801,17 @@
     </row>
     <row r="118" ht="12.75" customHeight="1">
       <c r="B118" s="301" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="119" ht="12.75" customHeight="1">
       <c r="B119" s="301" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="120" ht="12.75" customHeight="1">
       <c r="B120" s="301" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="121" ht="12.75" customHeight="1">
@@ -24825,7 +24821,7 @@
     </row>
     <row r="122" ht="12.75" customHeight="1">
       <c r="B122" s="301" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1">
@@ -25683,7 +25679,7 @@
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="B3" s="309" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C3" s="276"/>
       <c r="D3" s="276"/>
@@ -25706,13 +25702,13 @@
         <v>69</v>
       </c>
       <c r="C5" s="312" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D5" s="312" t="s">
         <v>400</v>
       </c>
       <c r="E5" s="312" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" ht="27.75" customHeight="1">
@@ -25721,13 +25717,13 @@
         <v>1.0</v>
       </c>
       <c r="C6" s="314" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D6" s="315" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E6" s="313" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -25757,13 +25753,13 @@
         <v>2.0</v>
       </c>
       <c r="C7" s="316" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D7" s="317" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E7" s="313" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -25793,13 +25789,13 @@
         <v>3.0</v>
       </c>
       <c r="C8" s="316" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D8" s="317" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E8" s="313" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F8" s="318"/>
       <c r="G8" s="318"/>
@@ -25829,13 +25825,13 @@
         <v>4.0</v>
       </c>
       <c r="C9" s="316" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D9" s="317" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E9" s="313" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F9" s="318"/>
       <c r="G9" s="318"/>
@@ -25865,13 +25861,13 @@
         <v>5.0</v>
       </c>
       <c r="C10" s="316" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D10" s="317" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E10" s="313" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F10" s="318"/>
       <c r="G10" s="318"/>
@@ -25901,13 +25897,13 @@
         <v>6.0</v>
       </c>
       <c r="C11" s="316" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D11" s="317" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E11" s="313" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F11" s="318"/>
       <c r="G11" s="318"/>
@@ -25937,13 +25933,13 @@
         <v>7.0</v>
       </c>
       <c r="C12" s="316" t="s">
+        <v>489</v>
+      </c>
+      <c r="D12" s="317" t="s">
+        <v>490</v>
+      </c>
+      <c r="E12" s="313" t="s">
         <v>488</v>
-      </c>
-      <c r="D12" s="317" t="s">
-        <v>489</v>
-      </c>
-      <c r="E12" s="313" t="s">
-        <v>487</v>
       </c>
       <c r="F12" s="318"/>
       <c r="G12" s="318"/>
@@ -25973,13 +25969,13 @@
         <v>8.0</v>
       </c>
       <c r="C13" s="316" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D13" s="317" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E13" s="313" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F13" s="318"/>
       <c r="G13" s="318"/>
@@ -26009,13 +26005,13 @@
         <v>9.0</v>
       </c>
       <c r="C14" s="316" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D14" s="317" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E14" s="313" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F14" s="318"/>
       <c r="G14" s="318"/>
@@ -26045,13 +26041,13 @@
         <v>10.0</v>
       </c>
       <c r="C15" s="316" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D15" s="317" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E15" s="313" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F15" s="318"/>
       <c r="G15" s="318"/>
@@ -26081,13 +26077,13 @@
         <v>11.0</v>
       </c>
       <c r="C16" s="316" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D16" s="317" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E16" s="313" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F16" s="318"/>
       <c r="G16" s="318"/>

</xml_diff>